<commit_message>
fix issues with indexes
</commit_message>
<xml_diff>
--- a/exports/performance_run_1000.xlsx
+++ b/exports/performance_run_1000.xlsx
@@ -490,13 +490,13 @@
         <v>7</v>
       </c>
       <c r="D2" t="n">
-        <v>0.078</v>
+        <v>0.077</v>
       </c>
       <c r="E2" t="n">
+        <v>0.095</v>
+      </c>
+      <c r="F2" t="n">
         <v>0.08</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.078</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -520,13 +520,13 @@
         <v>7</v>
       </c>
       <c r="D3" t="n">
-        <v>0.044</v>
+        <v>0.042</v>
       </c>
       <c r="E3" t="n">
-        <v>0.05</v>
+        <v>0.14</v>
       </c>
       <c r="F3" t="n">
-        <v>0.045</v>
+        <v>0.062</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -550,13 +550,13 @@
         <v>7</v>
       </c>
       <c r="D4" t="n">
-        <v>0.008</v>
+        <v>0.007</v>
       </c>
       <c r="E4" t="n">
         <v>0.008</v>
       </c>
       <c r="F4" t="n">
-        <v>0.008</v>
+        <v>0.007</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -580,13 +580,13 @@
         <v>7</v>
       </c>
       <c r="D5" t="n">
-        <v>0.482</v>
+        <v>0.442</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5590000000000001</v>
+        <v>0.468</v>
       </c>
       <c r="F5" t="n">
-        <v>0.488</v>
+        <v>0.449</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -610,19 +610,19 @@
         <v>7</v>
       </c>
       <c r="D6" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.068</v>
       </c>
       <c r="E6" t="n">
-        <v>0.103</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="F6" t="n">
-        <v>0.082</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>546</v>
+        <v>532</v>
       </c>
     </row>
     <row r="7">
@@ -640,13 +640,13 @@
         <v>7</v>
       </c>
       <c r="D7" t="n">
-        <v>0.218</v>
+        <v>0.216</v>
       </c>
       <c r="E7" t="n">
-        <v>0.245</v>
+        <v>0.219</v>
       </c>
       <c r="F7" t="n">
-        <v>0.225</v>
+        <v>0.216</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -670,13 +670,13 @@
         <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>0.61</v>
+        <v>0.601</v>
       </c>
       <c r="E8" t="n">
-        <v>0.678</v>
+        <v>0.609</v>
       </c>
       <c r="F8" t="n">
-        <v>0.617</v>
+        <v>0.592</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -700,19 +700,19 @@
         <v>7</v>
       </c>
       <c r="D9" t="n">
-        <v>0.372</v>
+        <v>0.299</v>
       </c>
       <c r="E9" t="n">
-        <v>0.411</v>
+        <v>0.326</v>
       </c>
       <c r="F9" t="n">
-        <v>0.384</v>
+        <v>0.309</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>924</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="10">
@@ -730,19 +730,19 @@
         <v>7</v>
       </c>
       <c r="D10" t="n">
-        <v>0.402</v>
+        <v>0.295</v>
       </c>
       <c r="E10" t="n">
-        <v>0.443</v>
+        <v>0.327</v>
       </c>
       <c r="F10" t="n">
-        <v>0.412</v>
+        <v>0.306</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>665</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="11">
@@ -760,13 +760,13 @@
         <v>7</v>
       </c>
       <c r="D11" t="n">
-        <v>0.636</v>
+        <v>0.837</v>
       </c>
       <c r="E11" t="n">
-        <v>0.664</v>
+        <v>1.679</v>
       </c>
       <c r="F11" t="n">
-        <v>0.624</v>
+        <v>0.994</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -790,13 +790,13 @@
         <v>7</v>
       </c>
       <c r="D12" t="n">
-        <v>0.31</v>
+        <v>0.313</v>
       </c>
       <c r="E12" t="n">
-        <v>0.37</v>
+        <v>0.329</v>
       </c>
       <c r="F12" t="n">
-        <v>0.326</v>
+        <v>0.314</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -820,13 +820,13 @@
         <v>7</v>
       </c>
       <c r="D13" t="n">
-        <v>0.276</v>
+        <v>0.263</v>
       </c>
       <c r="E13" t="n">
-        <v>0.356</v>
+        <v>0.345</v>
       </c>
       <c r="F13" t="n">
-        <v>0.293</v>
+        <v>0.282</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -850,13 +850,13 @@
         <v>7</v>
       </c>
       <c r="D14" t="n">
-        <v>0.223</v>
+        <v>0.21</v>
       </c>
       <c r="E14" t="n">
-        <v>0.343</v>
+        <v>0.232</v>
       </c>
       <c r="F14" t="n">
-        <v>0.251</v>
+        <v>0.214</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -880,13 +880,13 @@
         <v>7</v>
       </c>
       <c r="D15" t="n">
-        <v>0.779</v>
+        <v>0.757</v>
       </c>
       <c r="E15" t="n">
-        <v>0.8070000000000001</v>
+        <v>0.822</v>
       </c>
       <c r="F15" t="n">
-        <v>0.783</v>
+        <v>0.771</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
@@ -910,13 +910,13 @@
         <v>7</v>
       </c>
       <c r="D16" t="n">
-        <v>0.698</v>
+        <v>0.697</v>
       </c>
       <c r="E16" t="n">
-        <v>0.721</v>
+        <v>0.754</v>
       </c>
       <c r="F16" t="n">
-        <v>0.703</v>
+        <v>0.702</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
@@ -940,13 +940,13 @@
         <v>7</v>
       </c>
       <c r="D17" t="n">
-        <v>0.406</v>
+        <v>0.371</v>
       </c>
       <c r="E17" t="n">
-        <v>0.426</v>
+        <v>0.399</v>
       </c>
       <c r="F17" t="n">
-        <v>0.401</v>
+        <v>0.378</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
@@ -970,13 +970,13 @@
         <v>7</v>
       </c>
       <c r="D18" t="n">
-        <v>0.581</v>
+        <v>0.575</v>
       </c>
       <c r="E18" t="n">
-        <v>0.619</v>
+        <v>0.671</v>
       </c>
       <c r="F18" t="n">
-        <v>0.583</v>
+        <v>0.592</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
@@ -1000,19 +1000,19 @@
         <v>7</v>
       </c>
       <c r="D19" t="n">
-        <v>0.366</v>
+        <v>0.308</v>
       </c>
       <c r="E19" t="n">
-        <v>0.423</v>
+        <v>0.341</v>
       </c>
       <c r="F19" t="n">
-        <v>0.38</v>
+        <v>0.321</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>924</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="20">
@@ -1030,19 +1030,19 @@
         <v>7</v>
       </c>
       <c r="D20" t="n">
-        <v>0.412</v>
+        <v>0.307</v>
       </c>
       <c r="E20" t="n">
-        <v>0.468</v>
+        <v>0.336</v>
       </c>
       <c r="F20" t="n">
-        <v>0.426</v>
+        <v>0.316</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>665</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="21">
@@ -1060,13 +1060,13 @@
         <v>7</v>
       </c>
       <c r="D21" t="n">
-        <v>0.711</v>
+        <v>0.668</v>
       </c>
       <c r="E21" t="n">
-        <v>0.75</v>
+        <v>1.69</v>
       </c>
       <c r="F21" t="n">
-        <v>0.721</v>
+        <v>0.853</v>
       </c>
       <c r="G21" t="n">
         <v>0</v>
@@ -1090,13 +1090,13 @@
         <v>7</v>
       </c>
       <c r="D22" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="E22" t="n">
         <v>0.044</v>
       </c>
-      <c r="E22" t="n">
-        <v>0.063</v>
-      </c>
       <c r="F22" t="n">
-        <v>0.047</v>
+        <v>0.043</v>
       </c>
       <c r="G22" t="n">
         <v>0</v>
@@ -1123,10 +1123,10 @@
         <v>0.033</v>
       </c>
       <c r="E23" t="n">
-        <v>0.035</v>
+        <v>0.036</v>
       </c>
       <c r="F23" t="n">
-        <v>0.033</v>
+        <v>0.034</v>
       </c>
       <c r="G23" t="n">
         <v>0</v>
@@ -1153,10 +1153,10 @@
         <v>0.007</v>
       </c>
       <c r="E24" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.007</v>
       </c>
       <c r="F24" t="n">
-        <v>0.008</v>
+        <v>0.007</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
@@ -1180,13 +1180,13 @@
         <v>7</v>
       </c>
       <c r="D25" t="n">
-        <v>0.611</v>
+        <v>0.619</v>
       </c>
       <c r="E25" t="n">
-        <v>0.699</v>
+        <v>0.634</v>
       </c>
       <c r="F25" t="n">
-        <v>0.627</v>
+        <v>0.613</v>
       </c>
       <c r="G25" t="n">
         <v>0</v>
@@ -1213,16 +1213,16 @@
         <v>0.042</v>
       </c>
       <c r="E26" t="n">
-        <v>0.044</v>
+        <v>0.047</v>
       </c>
       <c r="F26" t="n">
-        <v>0.042</v>
+        <v>0.043</v>
       </c>
       <c r="G26" t="n">
         <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>329</v>
+        <v>336</v>
       </c>
     </row>
     <row r="27">
@@ -1240,13 +1240,13 @@
         <v>7</v>
       </c>
       <c r="D27" t="n">
-        <v>0.285</v>
+        <v>0.286</v>
       </c>
       <c r="E27" t="n">
-        <v>0.312</v>
+        <v>0.343</v>
       </c>
       <c r="F27" t="n">
-        <v>0.292</v>
+        <v>0.299</v>
       </c>
       <c r="G27" t="n">
         <v>0</v>
@@ -1270,13 +1270,13 @@
         <v>7</v>
       </c>
       <c r="D28" t="n">
-        <v>0.315</v>
+        <v>0.316</v>
       </c>
       <c r="E28" t="n">
-        <v>0.335</v>
+        <v>0.344</v>
       </c>
       <c r="F28" t="n">
-        <v>0.318</v>
+        <v>0.325</v>
       </c>
       <c r="G28" t="n">
         <v>0</v>
@@ -1300,13 +1300,13 @@
         <v>7</v>
       </c>
       <c r="D29" t="n">
-        <v>0.041</v>
+        <v>0.033</v>
       </c>
       <c r="E29" t="n">
-        <v>0.041</v>
+        <v>0.036</v>
       </c>
       <c r="F29" t="n">
-        <v>0.04</v>
+        <v>0.034</v>
       </c>
       <c r="G29" t="n">
         <v>0</v>
@@ -1330,13 +1330,13 @@
         <v>7</v>
       </c>
       <c r="D30" t="n">
-        <v>0.008</v>
+        <v>0.007</v>
       </c>
       <c r="E30" t="n">
-        <v>0.012</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="F30" t="n">
-        <v>0.008</v>
+        <v>0.007</v>
       </c>
       <c r="G30" t="n">
         <v>0</v>
@@ -1360,13 +1360,13 @@
         <v>7</v>
       </c>
       <c r="D31" t="n">
-        <v>0.233</v>
+        <v>0.241</v>
       </c>
       <c r="E31" t="n">
-        <v>0.265</v>
+        <v>0.272</v>
       </c>
       <c r="F31" t="n">
-        <v>0.241</v>
+        <v>0.246</v>
       </c>
       <c r="G31" t="n">
         <v>0</v>
@@ -1390,13 +1390,13 @@
         <v>7</v>
       </c>
       <c r="D32" t="n">
-        <v>0.119</v>
+        <v>0.115</v>
       </c>
       <c r="E32" t="n">
-        <v>0.147</v>
+        <v>0.117</v>
       </c>
       <c r="F32" t="n">
-        <v>0.128</v>
+        <v>0.115</v>
       </c>
       <c r="G32" t="n">
         <v>0</v>
@@ -1420,13 +1420,13 @@
         <v>7</v>
       </c>
       <c r="D33" t="n">
-        <v>0.217</v>
+        <v>0.212</v>
       </c>
       <c r="E33" t="n">
-        <v>0.243</v>
+        <v>0.235</v>
       </c>
       <c r="F33" t="n">
-        <v>0.225</v>
+        <v>0.216</v>
       </c>
       <c r="G33" t="n">
         <v>0</v>
@@ -1450,13 +1450,13 @@
         <v>7</v>
       </c>
       <c r="D34" t="n">
-        <v>0.11</v>
+        <v>0.107</v>
       </c>
       <c r="E34" t="n">
-        <v>0.15</v>
+        <v>0.107</v>
       </c>
       <c r="F34" t="n">
-        <v>0.118</v>
+        <v>0.107</v>
       </c>
       <c r="G34" t="n">
         <v>0</v>
@@ -1480,13 +1480,13 @@
         <v>7</v>
       </c>
       <c r="D35" t="n">
-        <v>0.626</v>
+        <v>0.629</v>
       </c>
       <c r="E35" t="n">
-        <v>0.966</v>
+        <v>0.66</v>
       </c>
       <c r="F35" t="n">
-        <v>0.6929999999999999</v>
+        <v>0.624</v>
       </c>
       <c r="G35" t="n">
         <v>0</v>
@@ -1510,13 +1510,13 @@
         <v>7</v>
       </c>
       <c r="D36" t="n">
-        <v>0.126</v>
+        <v>0.124</v>
       </c>
       <c r="E36" t="n">
-        <v>0.157</v>
+        <v>0.145</v>
       </c>
       <c r="F36" t="n">
-        <v>0.134</v>
+        <v>0.129</v>
       </c>
       <c r="G36" t="n">
         <v>0</v>
@@ -1540,13 +1540,13 @@
         <v>7</v>
       </c>
       <c r="D37" t="n">
-        <v>0.296</v>
+        <v>0.295</v>
       </c>
       <c r="E37" t="n">
-        <v>0.336</v>
+        <v>0.359</v>
       </c>
       <c r="F37" t="n">
-        <v>0.304</v>
+        <v>0.307</v>
       </c>
       <c r="G37" t="n">
         <v>0</v>
@@ -1570,13 +1570,13 @@
         <v>7</v>
       </c>
       <c r="D38" t="n">
-        <v>0.353</v>
+        <v>0.324</v>
       </c>
       <c r="E38" t="n">
-        <v>0.395</v>
+        <v>0.35</v>
       </c>
       <c r="F38" t="n">
-        <v>0.356</v>
+        <v>0.331</v>
       </c>
       <c r="G38" t="n">
         <v>0</v>
@@ -1603,10 +1603,10 @@
         <v>0.195</v>
       </c>
       <c r="E39" t="n">
-        <v>0.215</v>
+        <v>0.196</v>
       </c>
       <c r="F39" t="n">
-        <v>0.199</v>
+        <v>0.194</v>
       </c>
       <c r="G39" t="n">
         <v>0</v>
@@ -1630,13 +1630,13 @@
         <v>7</v>
       </c>
       <c r="D40" t="n">
+        <v>0.194</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.196</v>
+      </c>
+      <c r="F40" t="n">
         <v>0.195</v>
-      </c>
-      <c r="E40" t="n">
-        <v>0.235</v>
-      </c>
-      <c r="F40" t="n">
-        <v>0.205</v>
       </c>
       <c r="G40" t="n">
         <v>0</v>
@@ -1660,13 +1660,13 @@
         <v>7</v>
       </c>
       <c r="D41" t="n">
-        <v>0.243</v>
+        <v>0.241</v>
       </c>
       <c r="E41" t="n">
-        <v>0.261</v>
+        <v>0.262</v>
       </c>
       <c r="F41" t="n">
-        <v>0.246</v>
+        <v>0.245</v>
       </c>
       <c r="G41" t="n">
         <v>0</v>

</xml_diff>